<commit_message>
Medication administration to correct flow
</commit_message>
<xml_diff>
--- a/ExcelFiles/PharmacyPortal.xlsx
+++ b/ExcelFiles/PharmacyPortal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4ClinicalAuto\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B082735-43DD-4538-BD40-0D8E51AE2F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDAA89F-DA3D-494F-8B51-869082428C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>saurabh.c4</t>
-  </si>
-  <si>
     <t>Saurabh@202526</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>For Testing</t>
+  </si>
+  <si>
+    <t>trainer.saurabh</t>
   </si>
 </sst>
 </file>
@@ -594,17 +594,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,12 +610,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -636,268 +634,269 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" style="1" customWidth="1"/>
     <col min="4" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="1" customWidth="1"/>
-    <col min="23" max="27" width="9.140625" style="1"/>
-    <col min="28" max="28" width="12.7109375" style="1" customWidth="1"/>
-    <col min="29" max="40" width="9.140625" style="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1796875" style="1"/>
+    <col min="21" max="21" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.26953125" style="1" customWidth="1"/>
+    <col min="23" max="27" width="9.1796875" style="1"/>
+    <col min="28" max="28" width="12.7265625" style="1" customWidth="1"/>
+    <col min="29" max="40" width="9.1796875" style="1"/>
+    <col min="41" max="41" width="8.7265625" customWidth="1"/>
+    <col min="42" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>40</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>41</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>44</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>45</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>46</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>47</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>48</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>50</v>
       </c>
-      <c r="AV1" t="s">
+    </row>
+    <row r="2" spans="1:48" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:48" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="W2" s="1">
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y2" s="1">
         <v>0</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AI2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AM2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="5" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pharmacy portal. Current changes. Flow done  up to dispensing prescription
</commit_message>
<xml_diff>
--- a/ExcelFiles/PharmacyPortal.xlsx
+++ b/ExcelFiles/PharmacyPortal.xlsx
@@ -8,25 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4ClinicalAuto\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDAA89F-DA3D-494F-8B51-869082428C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E1F528-6156-4BA7-9694-0AA675A5D16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
     <sheet name="addPatient" sheetId="2" r:id="rId2"/>
+    <sheet name="AddMedication" sheetId="3" r:id="rId3"/>
+    <sheet name="EditMedication" sheetId="5" r:id="rId4"/>
+    <sheet name="AddPrescription" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="155">
   <si>
     <t>username</t>
   </si>
@@ -34,9 +51,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>Saurabh@202526</t>
-  </si>
-  <si>
     <t>pat_ethnicity_cod_id</t>
   </si>
   <si>
@@ -181,24 +195,9 @@
     <t>pat_disability_note</t>
   </si>
   <si>
-    <t>href05Reco005</t>
-  </si>
-  <si>
-    <t>B/O</t>
-  </si>
-  <si>
-    <t>Youk</t>
-  </si>
-  <si>
-    <t>Pawar</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>28/09/1994</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
@@ -250,25 +249,278 @@
     <t>For Testing</t>
   </si>
   <si>
-    <t>trainer.saurabh</t>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>pacr_category</t>
+  </si>
+  <si>
+    <t>pacr_que_name</t>
+  </si>
+  <si>
+    <t>medi_dose</t>
+  </si>
+  <si>
+    <t>medi_form</t>
+  </si>
+  <si>
+    <t>medi_frequency</t>
+  </si>
+  <si>
+    <t>medi_method</t>
+  </si>
+  <si>
+    <t>medi_route</t>
+  </si>
+  <si>
+    <t>medi_duration</t>
+  </si>
+  <si>
+    <t>meded_value</t>
+  </si>
+  <si>
+    <t>medi_start_date</t>
+  </si>
+  <si>
+    <t>medi_stop_date</t>
+  </si>
+  <si>
+    <t>pacr_status</t>
+  </si>
+  <si>
+    <t>pacr_risk</t>
+  </si>
+  <si>
+    <t>medi_dispensed</t>
+  </si>
+  <si>
+    <t>medi_prescribed_by</t>
+  </si>
+  <si>
+    <t>pcl_location_name</t>
+  </si>
+  <si>
+    <t>pacr_que_name_Diagnosis</t>
+  </si>
+  <si>
+    <t>medi_notes</t>
+  </si>
+  <si>
+    <t>medi_stopped_reason_eli_text</t>
+  </si>
+  <si>
+    <t>mse_text</t>
+  </si>
+  <si>
+    <t>paprd_endorsement</t>
+  </si>
+  <si>
+    <t>paprd_cost</t>
+  </si>
+  <si>
+    <t>meded_value_Price_check_quantity</t>
+  </si>
+  <si>
+    <t>meded_value_Administrator</t>
+  </si>
+  <si>
+    <t>meded_value_PGD</t>
+  </si>
+  <si>
+    <t>meded_value_MaxReffills</t>
+  </si>
+  <si>
+    <t>meded_value_Unit</t>
+  </si>
+  <si>
+    <t>meded_value_Quantity</t>
+  </si>
+  <si>
+    <t>meded_value_Adherent</t>
+  </si>
+  <si>
+    <t>eli_text</t>
+  </si>
+  <si>
+    <t>que_display_text</t>
+  </si>
+  <si>
+    <t>question_name</t>
+  </si>
+  <si>
+    <t>medadt_medication_status</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Paracetamol 500mg / Ibuprofen 200mg tablets</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>Oral</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>06/07/2025</t>
+  </si>
+  <si>
+    <t>08/07/2025</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Added notes for testing</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>PGD</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Adherent</t>
+  </si>
+  <si>
+    <t>Antibacterial</t>
+  </si>
+  <si>
+    <t>Dirty living conditions</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>given</t>
+  </si>
+  <si>
+    <t>s.d</t>
+  </si>
+  <si>
+    <t>Saurabh@2025</t>
+  </si>
+  <si>
+    <t>At Afternoon</t>
+  </si>
+  <si>
+    <t>Nausea</t>
+  </si>
+  <si>
+    <t>Adverse Reaction</t>
+  </si>
+  <si>
+    <t>Prescriber</t>
+  </si>
+  <si>
+    <t>Cardio 1</t>
+  </si>
+  <si>
+    <t>23/06/1982</t>
+  </si>
+  <si>
+    <t>href05Reco011</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>papre_code</t>
+  </si>
+  <si>
+    <t>12348765</t>
+  </si>
+  <si>
+    <t>pre_type</t>
+  </si>
+  <si>
+    <t>OP prescription</t>
+  </si>
+  <si>
+    <t>pre_notes</t>
+  </si>
+  <si>
+    <t>add for testing</t>
+  </si>
+  <si>
+    <t>medi_status</t>
+  </si>
+  <si>
+    <t>medi_risk</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Prescribed</t>
+  </si>
+  <si>
+    <t>Hospital consultant</t>
+  </si>
+  <si>
+    <t>Updated notes for testing</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>PSD</t>
+  </si>
+  <si>
+    <t>Edited notes for testing</t>
+  </si>
+  <si>
+    <t>Twice a  day</t>
+  </si>
+  <si>
+    <t>12/06/2026</t>
+  </si>
+  <si>
+    <t>14/06/2026</t>
+  </si>
+  <si>
+    <t>Insomnia</t>
+  </si>
+  <si>
+    <t>Cardio 2</t>
+  </si>
+  <si>
+    <t>PharmPatientP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,11 +543,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -303,17 +554,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -327,6 +578,168 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="loginDetails"/>
+      <sheetName val="PatientDetails"/>
+      <sheetName val="MedicationCategory"/>
+      <sheetName val="AddMedication"/>
+      <sheetName val="EditMedication"/>
+      <sheetName val="DeleteMedication"/>
+      <sheetName val="MedicationEDS"/>
+      <sheetName val="AddExamination"/>
+      <sheetName val="EditExamination"/>
+      <sheetName val="DeleteExamination"/>
+      <sheetName val="AddRecommendations"/>
+      <sheetName val="EditRecommendations"/>
+      <sheetName val="DeleteRecommendations"/>
+      <sheetName val="AddOutcome"/>
+      <sheetName val="EditOutcome"/>
+      <sheetName val="DeleteOutcome"/>
+      <sheetName val="AddDiagnosis"/>
+      <sheetName val="EditDiagnosis"/>
+      <sheetName val="DeleteDiagnosis"/>
+      <sheetName val="AddInterpretation"/>
+      <sheetName val="EditInterpretation"/>
+      <sheetName val="DeleteInterpretation"/>
+      <sheetName val="AddAllergy"/>
+      <sheetName val="EditAllergy"/>
+      <sheetName val="DeleteAllergy"/>
+      <sheetName val="AddProcedure"/>
+      <sheetName val="EditProcedure"/>
+      <sheetName val="DeleteProcedure"/>
+      <sheetName val="AddPatientScan"/>
+      <sheetName val="EditPatientScan"/>
+      <sheetName val="DeletePatientScan"/>
+      <sheetName val="AddProblems"/>
+      <sheetName val="EditProblems"/>
+      <sheetName val="DeleteProblems"/>
+      <sheetName val="AddOverview"/>
+      <sheetName val="EditOverview"/>
+      <sheetName val="DeleteOverview"/>
+      <sheetName val="Addsocial"/>
+      <sheetName val="Editsocial"/>
+      <sheetName val="Deletesocial"/>
+      <sheetName val="AddRiskFactor"/>
+      <sheetName val="EditRiskFactor"/>
+      <sheetName val="DeleteRiskFactor"/>
+      <sheetName val="AddLifestyle"/>
+      <sheetName val="EditLifestyle"/>
+      <sheetName val="DeleteLifestyle"/>
+      <sheetName val="AddInvestigation"/>
+      <sheetName val="EditInvestigation"/>
+      <sheetName val="AddCondition"/>
+      <sheetName val="EditCondition"/>
+      <sheetName val="DeleteCondition"/>
+      <sheetName val="AddPatientDetails"/>
+      <sheetName val="EditPatientDetails"/>
+      <sheetName val="DeletePatientDetails"/>
+      <sheetName val="AddTask"/>
+      <sheetName val="EditTask"/>
+      <sheetName val="AddCarePlan"/>
+      <sheetName val="EditCarePlan"/>
+      <sheetName val="DeleteCarePlan"/>
+      <sheetName val="Alerts"/>
+      <sheetName val="DeleteInvestigation"/>
+      <sheetName val="DevicePatientDetails"/>
+      <sheetName val="AddDevice"/>
+      <sheetName val="EditDevice"/>
+      <sheetName val="AddTest"/>
+      <sheetName val="EditTest"/>
+      <sheetName val="AddTool"/>
+      <sheetName val="EditTool"/>
+      <sheetName val="AddPatientConsent"/>
+      <sheetName val="EditPatientConsent"/>
+      <sheetName val="PhysicalSign"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Paracetamol 500mg / Ibuprofen 200mg tablets</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+      <sheetData sheetId="62" refreshError="1"/>
+      <sheetData sheetId="63" refreshError="1"/>
+      <sheetData sheetId="64" refreshError="1"/>
+      <sheetData sheetId="65" refreshError="1"/>
+      <sheetData sheetId="66" refreshError="1"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
+      <sheetData sheetId="69" refreshError="1"/>
+      <sheetData sheetId="70" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -611,11 +1024,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
+      <c r="A2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -630,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BEABD6-BAD9-4B4F-B282-9FCE52D49032}">
   <dimension ref="A1:AV5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,241 +1076,712 @@
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>42</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>43</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>44</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>45</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>46</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>47</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>48</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>49</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="W2" s="1">
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="1">
         <v>0</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E97EB8-CC20-428F-9B49-9E02ADAD0F2B}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" t="s">
+        <v>128</v>
+      </c>
+      <c r="T2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="X2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC2">
+        <v>5</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E5DE0D-E686-4FAF-9854-B0387D320519}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="str">
+        <f>[1]AddMedication!B2</f>
+        <v>Paracetamol 500mg / Ibuprofen 200mg tablets</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P2" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="U2" t="s">
+        <v>147</v>
+      </c>
+      <c r="V2" t="s">
+        <v>148</v>
+      </c>
+      <c r="W2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B724E05-6618-48C8-A63A-0BA1FA2211F7}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pharmacy portal flow changes.
</commit_message>
<xml_diff>
--- a/ExcelFiles/PharmacyPortal.xlsx
+++ b/ExcelFiles/PharmacyPortal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4ClinicalAuto\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E1F528-6156-4BA7-9694-0AA675A5D16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E5DA2E-F44C-4324-939D-52E0F9463DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,9 @@
     <sheet name="addPatient" sheetId="2" r:id="rId2"/>
     <sheet name="AddMedication" sheetId="3" r:id="rId3"/>
     <sheet name="EditMedication" sheetId="5" r:id="rId4"/>
-    <sheet name="AddPrescription" sheetId="4" r:id="rId5"/>
+    <sheet name="DeleteMedication" sheetId="6" r:id="rId5"/>
+    <sheet name="AddPrescription" sheetId="4" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="157">
   <si>
     <t>username</t>
   </si>
@@ -354,9 +352,6 @@
     <t>Medication</t>
   </si>
   <si>
-    <t>Paracetamol 500mg / Ibuprofen 200mg tablets</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -435,9 +430,6 @@
     <t>Prescriber</t>
   </si>
   <si>
-    <t>Cardio 1</t>
-  </si>
-  <si>
     <t>23/06/1982</t>
   </si>
   <si>
@@ -489,9 +481,6 @@
     <t>PSD</t>
   </si>
   <si>
-    <t>Edited notes for testing</t>
-  </si>
-  <si>
     <t>Twice a  day</t>
   </si>
   <si>
@@ -507,7 +496,22 @@
     <t>Cardio 2</t>
   </si>
   <si>
-    <t>PharmPatientP</t>
+    <t>Paracetamol 500mg tablets</t>
+  </si>
+  <si>
+    <t>Cardio Location</t>
+  </si>
+  <si>
+    <t>Orally</t>
+  </si>
+  <si>
+    <t>pacr_delete_reason</t>
+  </si>
+  <si>
+    <t>Delete for testing</t>
+  </si>
+  <si>
+    <t>PharmPatientBG</t>
   </si>
 </sst>
 </file>
@@ -578,168 +582,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="loginDetails"/>
-      <sheetName val="PatientDetails"/>
-      <sheetName val="MedicationCategory"/>
-      <sheetName val="AddMedication"/>
-      <sheetName val="EditMedication"/>
-      <sheetName val="DeleteMedication"/>
-      <sheetName val="MedicationEDS"/>
-      <sheetName val="AddExamination"/>
-      <sheetName val="EditExamination"/>
-      <sheetName val="DeleteExamination"/>
-      <sheetName val="AddRecommendations"/>
-      <sheetName val="EditRecommendations"/>
-      <sheetName val="DeleteRecommendations"/>
-      <sheetName val="AddOutcome"/>
-      <sheetName val="EditOutcome"/>
-      <sheetName val="DeleteOutcome"/>
-      <sheetName val="AddDiagnosis"/>
-      <sheetName val="EditDiagnosis"/>
-      <sheetName val="DeleteDiagnosis"/>
-      <sheetName val="AddInterpretation"/>
-      <sheetName val="EditInterpretation"/>
-      <sheetName val="DeleteInterpretation"/>
-      <sheetName val="AddAllergy"/>
-      <sheetName val="EditAllergy"/>
-      <sheetName val="DeleteAllergy"/>
-      <sheetName val="AddProcedure"/>
-      <sheetName val="EditProcedure"/>
-      <sheetName val="DeleteProcedure"/>
-      <sheetName val="AddPatientScan"/>
-      <sheetName val="EditPatientScan"/>
-      <sheetName val="DeletePatientScan"/>
-      <sheetName val="AddProblems"/>
-      <sheetName val="EditProblems"/>
-      <sheetName val="DeleteProblems"/>
-      <sheetName val="AddOverview"/>
-      <sheetName val="EditOverview"/>
-      <sheetName val="DeleteOverview"/>
-      <sheetName val="Addsocial"/>
-      <sheetName val="Editsocial"/>
-      <sheetName val="Deletesocial"/>
-      <sheetName val="AddRiskFactor"/>
-      <sheetName val="EditRiskFactor"/>
-      <sheetName val="DeleteRiskFactor"/>
-      <sheetName val="AddLifestyle"/>
-      <sheetName val="EditLifestyle"/>
-      <sheetName val="DeleteLifestyle"/>
-      <sheetName val="AddInvestigation"/>
-      <sheetName val="EditInvestigation"/>
-      <sheetName val="AddCondition"/>
-      <sheetName val="EditCondition"/>
-      <sheetName val="DeleteCondition"/>
-      <sheetName val="AddPatientDetails"/>
-      <sheetName val="EditPatientDetails"/>
-      <sheetName val="DeletePatientDetails"/>
-      <sheetName val="AddTask"/>
-      <sheetName val="EditTask"/>
-      <sheetName val="AddCarePlan"/>
-      <sheetName val="EditCarePlan"/>
-      <sheetName val="DeleteCarePlan"/>
-      <sheetName val="Alerts"/>
-      <sheetName val="DeleteInvestigation"/>
-      <sheetName val="DevicePatientDetails"/>
-      <sheetName val="AddDevice"/>
-      <sheetName val="EditDevice"/>
-      <sheetName val="AddTest"/>
-      <sheetName val="EditTest"/>
-      <sheetName val="AddTool"/>
-      <sheetName val="EditTool"/>
-      <sheetName val="AddPatientConsent"/>
-      <sheetName val="EditPatientConsent"/>
-      <sheetName val="PhysicalSign"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Paracetamol 500mg / Ibuprofen 200mg tablets</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,10 +867,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
         <v>124</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1222,22 +1064,22 @@
     </row>
     <row r="2" spans="1:48" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>51</v>
@@ -1319,45 +1161,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E97EB8-CC20-428F-9B49-9E02ADAD0F2B}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
@@ -1469,97 +1312,97 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" t="s">
+        <v>112</v>
+      </c>
+      <c r="S2" t="s">
+        <v>127</v>
+      </c>
+      <c r="T2" t="s">
         <v>126</v>
       </c>
-      <c r="F2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="L2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O2" t="s">
-        <v>111</v>
-      </c>
-      <c r="P2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="X2" t="s">
         <v>128</v>
       </c>
-      <c r="T2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" s="4" t="s">
+      <c r="Y2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA2" t="s">
         <v>116</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="X2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="AC2">
         <v>5</v>
       </c>
       <c r="AD2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AE2" t="s">
         <v>119</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>120</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" t="s">
         <v>122</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1569,16 +1412,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E5DE0D-E686-4FAF-9854-B0387D320519}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
@@ -1594,15 +1437,14 @@
     <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1637,10 +1479,10 @@
         <v>79</v>
       </c>
       <c r="L1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N1" t="s">
         <v>82</v>
@@ -1667,76 +1509,70 @@
         <v>93</v>
       </c>
       <c r="V1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>102</v>
       </c>
       <c r="B2" t="str">
-        <f>[1]AddMedication!B2</f>
-        <v>Paracetamol 500mg / Ibuprofen 200mg tablets</v>
+        <f>AddMedication!B2</f>
+        <v>Paracetamol 500mg tablets</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" t="s">
         <v>149</v>
       </c>
-      <c r="F2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="S2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="U2" t="s">
+        <v>145</v>
+      </c>
+      <c r="V2" t="s">
         <v>150</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" t="s">
-        <v>143</v>
-      </c>
-      <c r="O2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P2" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>120</v>
-      </c>
-      <c r="R2" t="s">
-        <v>152</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="U2" t="s">
-        <v>147</v>
-      </c>
-      <c r="V2" t="s">
-        <v>148</v>
-      </c>
-      <c r="W2" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1745,6 +1581,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EE1E1A-F975-4FCE-AC16-98690042CE9C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="str">
+        <f>EditMedication!B2</f>
+        <v>Paracetamol 500mg tablets</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B724E05-6618-48C8-A63A-0BA1FA2211F7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1761,24 +1638,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
         <v>135</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>